<commit_message>
time left for auction added
</commit_message>
<xml_diff>
--- a/results/6800xt.xlsx
+++ b/results/6800xt.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>Purchase Options</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Time Left</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -491,7 +496,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/334664407065?hash=item4deb8d9819:g:FKIAAOSwnVBjmHe-&amp;amdata=enc%3AAQAHAAAAoCG5TsTwv3NrcsAMph23YpyOzpjg%2FazSUpiMv3ki3a%2F8bALlhsRZMiG0JBsmN6I%2FCrvEnKwLrsaLRtA7f67GxqiWW%2BLglRSFpMIm%2BeeDU6v3MAXGnr2VqnHINhmhYT4%2F3uqtSSzBuEZEg%2F%2FHU5H9jK7WwBoWYIXLze7Ql%2Be0ZEorI4SCV18djxFW%2FNzmuw4HM8fUrGGT1N%2BY9qKFSpt3J8U%3D%7Ctkp%3ABk9SR8b2yYOjYQ</t>
+          <t>https://www.ebay.com/itm/334664407065?hash=item4deb8d9819:g:FKIAAOSwnVBjmHe-&amp;amdata=enc%3AAQAHAAAAoCG5TsTwv3NrcsAMph23YpyOzpjg%2FazSUpiMv3ki3a%2F8FVgE5ZK4lZIiQGyAC%2FdZ4xGQCBq3%2FmamHjwsFXxsfaUPLZ1sFmtJUXDunazGVqfFrr53b7Olk3lu9gylYT9DJgSxOvup5%2BkvNA859qS20gbDjdMJ6U8RU9SnjTuGxZi7G4vsWVnfwK2CQw3yM%2FnNxux1K%2Fe6QjyIyJEepHrwvJk%3D%7Ctkp%3ABk9SR8C8t7WjYQ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -521,6 +526,11 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>ou Oferta direta</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Not specified</t>
         </is>
       </c>
     </row>
@@ -535,7 +545,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/385163444573?epid=23050214728&amp;hash=item59ad87c15d:g:oFAAAOSw5yxjRIsG&amp;amdata=enc%3AAQAHAAAAoHHTmOg%2BoR3LtRCMXYQ8lAEEmjWes9DhmmiUWq2HMpjVm3mECPsrpnLZ8kWNFz9IUgtqkuqEQ7psEgog4%2BOI6knBUIyca%2Fxr1C2MPbR7luKL%2FH%2FQGIMFoJTpFCFwUmUQ6bHaJGHsBH%2FnYWEYmxOq53V7xXNsoYBLlAxY%2FZI9Omfk8iPZrtaXpS%2B3u%2FfXjRRPZNOsZdGzDHIgaSRucpX7Mzw%3D%7Ctkp%3ABk9SR8b2yYOjYQ</t>
+          <t>https://www.ebay.com/itm/385163444573?epid=23050214728&amp;hash=item59ad87c15d:g:oFAAAOSw5yxjRIsG&amp;amdata=enc%3AAQAHAAAAoHHTmOg%2BoR3LtRCMXYQ8lAEEmjWes9DhmmiUWq2HMpjVVk%2FNDA2W4sdxSIQ5obiJZQz00dOOV%2FK5RwnOY3%2B7GF1HujRXbDUY7TxyD3o%2Fh4cwR6khxppUTdNw74CKaC%2FPwZHdFpdhHZmEnu29pPOZ9yGbKa501U6N703auECAI5PIi6s5BTezv1fm3sviBmhA0FvuvbQm0K26sjHtryL3Fmk%3D%7Ctkp%3ABk9SR8K8t7WjYQ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -565,6 +575,11 @@
       <c r="J3" t="inlineStr">
         <is>
           <t>ou Oferta direta</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Not specified</t>
         </is>
       </c>
     </row>
@@ -579,7 +594,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/364076525731?hash=item54c4a6e8a3:g:JX4AAOSw~CJjlfzi&amp;amdata=enc%3AAQAHAAAA4NEFSvBjjHf1HqZEVcXoZ9YLAa73ryw5jSNYF2sLOSWID%2BxtVxTnPABtjH8Nei4mTWgNSGZjxqr1ZTELd%2F93QaV%2FGDqedav6ALUeZag8TKyPVwVofWZy2%2FNUuRdaPYQDwLh1zkYYIsLJURJ4w9nVesbT%2BFs%2Bflj2oM9ND0ECGXPDeRQP0TYRkcZTCC%2BGvBZBOMEiIh6RxtUmQatJPq304awGIq6tzmhOoCKQqPgx9U%2FmrmBeBcOCfxVDdnD9hgVXp%2F1XdPgb%2BqtwD1%2FXmobBvJuV%2Bx7XdnW%2FKn8e0i2xkME7%7Ctkp%3ABk9SR8b2yYOjYQ</t>
+          <t>https://www.ebay.com/itm/364076525731?hash=item54c4a6e8a3:g:JX4AAOSw~CJjlfzi&amp;amdata=enc%3AAQAHAAAA4NEFSvBjjHf1HqZEVcXoZ9aEHAWu9bZtDogcLQ1aECJrJ4bqtAM2GcxfCgyJWBDbzJoIrzPMG0Cg7y%2BGOVailhMwXU4A7A09ESoKAM2JBOuXId253o%2F8uJGTEwKxMubxgfIgbB4jdrxHgk4q3WP7JKDvqFgkqWEHx0YOfpund8EmW30IjJIoBYFcvZx2%2B05boDpcuS%2BeVKLgZsfaWoVIV3gJubhgvE%2Fa8RjnHdJuEZhdmNu6sd9mMVAM4Q8w3p6hTzQCIkbucd4yHGzo8%2B%2FjPKdw0sVBzXJMx8oBJbkNGNQR%7Ctkp%3ABk9SR8C8t7WjYQ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -588,7 +603,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>421</v>
+        <v>450</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -599,7 +614,7 @@
         <v>15</v>
       </c>
       <c r="H4" t="n">
-        <v>436</v>
+        <v>465</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -609,6 +624,11 @@
       <c r="J4" t="inlineStr">
         <is>
           <t>No other purchase options</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2d 1h restantes</t>
         </is>
       </c>
     </row>
@@ -623,7 +643,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/155308020238?hash=item242914520e:g:HecAAOSw6CBjmLE8&amp;amdata=enc%3AAQAHAAAAkINXBQ6TDT7aR4w2cDXsHla8%2F9Ul%2FpYukvcoYW7Eov4CGZNERvDstq4EvOXTP7DN6KXkG%2FW3U%2BF%2BcXMnBUETh5LwZsWJs8b1nxAscN21uHcDakCU1ftK%2BPa2js5U%2Bp0cCP9tVy2kX9Rh%2FB9KTOEIPddaR1qrr6FcjAP%2Fo0dBlaC8h0bGtvHdS%2FDU3IeGQvH%2BjA%3D%3D%7Ctkp%3ABk9SR8b2yYOjYQ</t>
+          <t>https://www.ebay.com/itm/155308020238?hash=item242914520e:g:HecAAOSw6CBjmLE8&amp;amdata=enc%3AAQAHAAAAkINXBQ6TDT7aR4w2cDXsHla8%2F9Ul%2FpYukvcoYW7Eov4CrBmSjpfukU7mosoB2HqrTVLki2AttJRfLQmk4wQb%2BfDKJ4WiKr46Fc3erFfTH0FAEZJ%2BjBTl7ycxS3IXvsu0bHOUmPBmTmS%2FRBlcU2zxbwJkr9BFfARP0WC8nRTKDdGxCcRDVTgaLZ0Id2mmtsRjrA%3D%3D%7Ctkp%3ABk9SR8C8t7WjYQ</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -632,7 +652,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -643,7 +663,7 @@
         <v>15</v>
       </c>
       <c r="H5" t="n">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -653,6 +673,11 @@
       <c r="J5" t="inlineStr">
         <is>
           <t>No other purchase options</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2d 2h restantes</t>
         </is>
       </c>
     </row>
@@ -667,7 +692,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/175531638048?hash=item28de803d20:g:1rwAAOSwGZ5jjxIj&amp;amdata=enc%3AAQAHAAAAkDUDHPwW2TkeJpPu0PLgguIKqM6OK8we5QyqR8AY203rnbE%2BQrLbmFkJ8NiOoHngltleYSapiqraQ%2BGEGQblqo5V%2BsICo5Om%2FjdGdseAK2%2B1aMXLAzVa68gNTB7faVazHI9RPmnse%2FTWtRYaFzH1k1ykd8uVMD6%2F6rvLZ6Q69D55Wbh6lCTjyaSjHOxHIOIBKg%3D%3D%7Ctkp%3ABk9SR8b2yYOjYQ</t>
+          <t>https://www.ebay.com/itm/175531638048?hash=item28de803d20:g:1rwAAOSwGZ5jjxIj&amp;amdata=enc%3AAQAHAAAAkDUDHPwW2TkeJpPu0PLgguIKqM6OK8we5QyqR8AY203rTSvKqOyw6cxUU5TxcD25ytKRn5wIIAvNEsx%2Fua6UFblJPEmstQdP5a8RMKu9eMouJp0Chy9jf8qtXa86zTXO%2BHdjAqNn%2FpfUBS6jA1OCgMt57G%2F5BBQ2GMK9cAJjrIEA%2F0fLGXYewAECtRQGzVCWzg%3D%3D%7Ctkp%3ABk9SR8K8t7WjYQ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -697,6 +722,11 @@
       <c r="J6" t="inlineStr">
         <is>
           <t>No other purchase options</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>3d 20h restantes</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
string distance metric was added
</commit_message>
<xml_diff>
--- a/results/6800xt.xlsx
+++ b/results/6800xt.xlsx
@@ -487,16 +487,16 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tarjeta gráfica AMD Radeon RX 6800 XT</t>
+          <t>AMD Radeon Rx 6800xt 16G Pcie 4.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/334664407065?hash=item4deb8d9819:g:FKIAAOSwnVBjmHe-&amp;amdata=enc%3AAQAHAAAAoCG5TsTwv3NrcsAMph23YpyOzpjg%2FazSUpiMv3ki3a%2F8FVgE5ZK4lZIiQGyAC%2FdZ4xGQCBq3%2FmamHjwsFXxsfaUPLZ1sFmtJUXDunazGVqfFrr53b7Olk3lu9gylYT9DJgSxOvup5%2BkvNA859qS20gbDjdMJ6U8RU9SnjTuGxZi7G4vsWVnfwK2CQw3yM%2FnNxux1K%2Fe6QjyIyJEepHrwvJk%3D%7Ctkp%3ABk9SR8C8t7WjYQ</t>
+          <t>https://www.ebay.com/itm/175531714780?hash=item28de8168dc:g:t0YAAOSwBbpjmF4E&amp;amdata=enc%3AAQAHAAAAoP4qtSmdnF7K6kKgCTQO2HJR52%2BBOgy%2BA%2FQHGLUkOvnoonZ9kbd%2BT08dcMptHax7gC%2BprXsM6AAI8ii5YMD7tw6n%2FtO%2FcMfxF%2Blcba81qJg4ifs1Eek5fSoq%2F3f6XNj08jtuJbQipNh1AHfxu5BFoKqxgqE2pyZufALb2N86QBX7ndCGJlHfKCs837lFkH1Dzh2RosD4Z%2FZvq8UayNlgw4U%3D%7Ctkp%3ABk9SR6iqv8WjYQ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>600</v>
+        <v>565</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
         <v>25</v>
       </c>
       <c r="H2" t="n">
-        <v>625</v>
+        <v>590</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -545,7 +545,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/385163444573?epid=23050214728&amp;hash=item59ad87c15d:g:oFAAAOSw5yxjRIsG&amp;amdata=enc%3AAQAHAAAAoHHTmOg%2BoR3LtRCMXYQ8lAEEmjWes9DhmmiUWq2HMpjVVk%2FNDA2W4sdxSIQ5obiJZQz00dOOV%2FK5RwnOY3%2B7GF1HujRXbDUY7TxyD3o%2Fh4cwR6khxppUTdNw74CKaC%2FPwZHdFpdhHZmEnu29pPOZ9yGbKa501U6N703auECAI5PIi6s5BTezv1fm3sviBmhA0FvuvbQm0K26sjHtryL3Fmk%3D%7Ctkp%3ABk9SR8K8t7WjYQ</t>
+          <t>https://www.ebay.com/itm/385163444573?epid=23050214728&amp;hash=item59ad87c15d:g:oFAAAOSw5yxjRIsG&amp;amdata=enc%3AAQAHAAAAoHHTmOg%2BoR3LtRCMXYQ8lAEEmjWes9DhmmiUWq2HMpjVj7cHG6OArdLFELfIpHbYXf%2FxvqhhQHI16MdjiGX6kObyLNflfSBpAixGObFlZPIjcOfiKrnYEzcbQ3NhsODrompGmh%2F9TnPL6rVWiH%2F4z%2BGgeGZn23lV0AsL3%2Bn%2BHb5b5%2BmGMfvoAiHHIZ3wCCWloN1MM%2B9v071%2BjQBFDA10B0s%3D%7Ctkp%3ABk9SR6iqv8WjYQ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/364076525731?hash=item54c4a6e8a3:g:JX4AAOSw~CJjlfzi&amp;amdata=enc%3AAQAHAAAA4NEFSvBjjHf1HqZEVcXoZ9aEHAWu9bZtDogcLQ1aECJrJ4bqtAM2GcxfCgyJWBDbzJoIrzPMG0Cg7y%2BGOVailhMwXU4A7A09ESoKAM2JBOuXId253o%2F8uJGTEwKxMubxgfIgbB4jdrxHgk4q3WP7JKDvqFgkqWEHx0YOfpund8EmW30IjJIoBYFcvZx2%2B05boDpcuS%2BeVKLgZsfaWoVIV3gJubhgvE%2Fa8RjnHdJuEZhdmNu6sd9mMVAM4Q8w3p6hTzQCIkbucd4yHGzo8%2B%2FjPKdw0sVBzXJMx8oBJbkNGNQR%7Ctkp%3ABk9SR8C8t7WjYQ</t>
+          <t>https://www.ebay.com/itm/364076525731?hash=item54c4a6e8a3:g:JX4AAOSw~CJjlfzi&amp;amdata=enc%3AAQAHAAAA4NEFSvBjjHf1HqZEVcXoZ9aEHAWu9bZtDogcLQ1aECJrJ4bqtAM2GcxfCgyJWBDbzJoIrzPMG0Cg7y%2BGOVailhMwXU4A7A09ESoKAM2JBOuXId253o%2F8uJGTEwKxMubxgRRQ33B60oIIfIMx3Ec2hn5I4WNrnkMOXgGZwWTZiRioF2abPA%2F%2BoOko23se95%2F6Oh8xhM6O4mxI7a3Tsxq9hVnxbxT%2FSHjOsudJm8D6BwbvIrMmxij2Ty0e4UznU2XJQydJRsov8IRvPYjb1HcWArAdo3YfvIE%2Fl4dg4iNfz88k%7Ctkp%3ABk9SR6iqv8WjYQ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -614,7 +614,7 @@
         <v>15</v>
       </c>
       <c r="H4" t="n">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -628,13 +628,13 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2d 1h restantes</t>
+          <t>1d 20h restantes</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -643,7 +643,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/155308020238?hash=item242914520e:g:HecAAOSw6CBjmLE8&amp;amdata=enc%3AAQAHAAAAkINXBQ6TDT7aR4w2cDXsHla8%2F9Ul%2FpYukvcoYW7Eov4CrBmSjpfukU7mosoB2HqrTVLki2AttJRfLQmk4wQb%2BfDKJ4WiKr46Fc3erFfTH0FAEZJ%2BjBTl7ycxS3IXvsu0bHOUmPBmTmS%2FRBlcU2zxbwJkr9BFfARP0WC8nRTKDdGxCcRDVTgaLZ0Id2mmtsRjrA%3D%3D%7Ctkp%3ABk9SR8C8t7WjYQ</t>
+          <t>https://www.ebay.com/itm/155308020238?hash=item242914520e:g:HecAAOSw6CBjmLE8&amp;amdata=enc%3AAQAHAAAAkINXBQ6TDT7aR4w2cDXsHla8%2F9Ul%2FpYukvcoYW7Eov4Cb4GvJmWTkx5qmIHfV0oZdazVqMWw23GMNqSOI35n6NV1iZnDB6D4YsX3gaVZKEuilkg303CshW7W6bHiny8HRZQa1EsmTT3oBK3AlIB%2BW%2Bh2KYyVY4mCHZO7I4MWGdZUBzVdje8cIy%2BwlEea%2BHuJTg%3D%3D%7Ctkp%3ABk9SR6iqv8WjYQ</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -677,7 +677,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2d 2h restantes</t>
+          <t>1d 22h restantes</t>
         </is>
       </c>
     </row>
@@ -692,7 +692,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/175531638048?hash=item28de803d20:g:1rwAAOSwGZ5jjxIj&amp;amdata=enc%3AAQAHAAAAkDUDHPwW2TkeJpPu0PLgguIKqM6OK8we5QyqR8AY203rTSvKqOyw6cxUU5TxcD25ytKRn5wIIAvNEsx%2Fua6UFblJPEmstQdP5a8RMKu9eMouJp0Chy9jf8qtXa86zTXO%2BHdjAqNn%2FpfUBS6jA1OCgMt57G%2F5BBQ2GMK9cAJjrIEA%2F0fLGXYewAECtRQGzVCWzg%3D%3D%7Ctkp%3ABk9SR8K8t7WjYQ</t>
+          <t>https://www.ebay.com/itm/175531638048?hash=item28de803d20:g:1rwAAOSwGZ5jjxIj&amp;amdata=enc%3AAQAHAAAAkDUDHPwW2TkeJpPu0PLgguIKqM6OK8we5QyqR8AY203rotyF%2Bfy4InheLSYDL5LLc9d3DYd3LHUgqYgGK8IGy5vKJ4mIijbeK0YIA426rAE2%2B626WktOUh3QdtVk5rLxiGE4lxeCUYdWxX%2F6ttQ3jyhHQWpmafQEfEuGL19D%2BfeY3etONS5bI3Epg5BMONOPWA%3D%3D%7Ctkp%3ABk9SR6iqv8WjYQ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>3d 20h restantes</t>
+          <t>3d 15h restantes</t>
         </is>
       </c>
     </row>

</xml_diff>